<commit_message>
Datos Diarios Energía Abierta CL
</commit_message>
<xml_diff>
--- a/Indicadores Diarios/Indicadores_Diarios.xlsx
+++ b/Indicadores Diarios/Indicadores_Diarios.xlsx
@@ -1233,7 +1233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C470"/>
+  <dimension ref="A1:C471"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9226,6 +9226,23 @@
         </is>
       </c>
       <c r="C470" t="inlineStr">
+        <is>
+          <t>Dolar</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>07-09-2021</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>770.33</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
         <is>
           <t>Dolar</t>
         </is>
@@ -9242,7 +9259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C470"/>
+  <dimension ref="A1:C471"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17235,6 +17252,23 @@
         </is>
       </c>
       <c r="C470" t="inlineStr">
+        <is>
+          <t>euro</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>07-09-2021</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>914.23</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
         <is>
           <t>euro</t>
         </is>

</xml_diff>